<commit_message>
Updated diagram, framework that includes additional calibratable parameters, and runnable calibration suggestions
</commit_message>
<xml_diff>
--- a/docs/tutorial/assets/T2/t2_databook_1.xlsx
+++ b/docs/tutorial/assets/T2/t2_databook_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\docs\tutorial\assets\T2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\atomica\docs\tutorial\assets\T2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B17E21-98CB-4BE4-8D3F-9753BE1B4AE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233AEFDD-3410-405B-BF15-47F4FE0EC7A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="4575" windowWidth="28785" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5055" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>Number of new infections</t>
+  </si>
+  <si>
+    <t>Number of deaths due to disease</t>
+  </si>
+  <si>
+    <t>Population size</t>
   </si>
 </sst>
 </file>
@@ -198,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -212,11 +221,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="17">
     <dxf>
       <fill>
         <patternFill patternType="lightUp">
@@ -231,6 +241,20 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="lightUp">
           <bgColor rgb="FFFF0000"/>
         </patternFill>
@@ -275,6 +299,37 @@
     <dxf>
       <fill>
         <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
       </fill>
     </dxf>
   </dxfs>
@@ -658,10 +713,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,8 +728,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
+      <c r="A1" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -688,7 +743,6 @@
       <c r="E1" s="1">
         <v>2020</v>
       </c>
-      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
@@ -700,15 +754,15 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="E2" s="2">
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -722,6 +776,7 @@
       <c r="E4" s="1">
         <v>2020</v>
       </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
@@ -733,13 +788,53 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="2">
         <v>500</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E8" s="2">
+        <v>800</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="expression" dxfId="16" priority="1">
+      <formula>AND(XFD1&lt;&gt;"",NOT(A1&lt;&gt;""))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B5" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5 B8 B2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Number"</formula1>
     </dataValidation>
   </dataValidations>
@@ -753,10 +848,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,49 +1098,157 @@
       </c>
       <c r="G15" s="2"/>
     </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
+        <v>2010</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="2">
+        <v>100</v>
+      </c>
+      <c r="G18" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1">
+        <v>2010</v>
+      </c>
+      <c r="G20" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="2">
+        <v>40</v>
+      </c>
+      <c r="G21" s="2">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>COUNTIF(F11:G11,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>AND(COUNTIF(F11:G11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="expression" dxfId="13" priority="15">
+      <formula>COUNTIF(F15:G15,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="16">
+      <formula>AND(COUNTIF(F15:G15,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="expression" dxfId="11" priority="7">
+      <formula>COUNTIF(F2:G2,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="8">
+      <formula>AND(COUNTIF(F2:G2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="expression" dxfId="9" priority="9">
+      <formula>COUNTIF(F5:G5,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="10">
+      <formula>AND(COUNTIF(F5:G5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="expression" dxfId="7" priority="11">
+      <formula>COUNTIF(F8:G8,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="12">
+      <formula>AND(COUNTIF(F8:G8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="7" priority="9">
-      <formula>COUNTIF(F15:G15,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="10">
-      <formula>AND(COUNTIF(F15:G15,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D15)))</formula>
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>COUNTIF(F12:G12,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>AND(COUNTIF(F12:G12,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="5" priority="1">
-      <formula>COUNTIF(F2:G2,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
-      <formula>AND(COUNTIF(F2:G2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D2)))</formula>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>AND(XFD17&lt;&gt;"",NOT(A17&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>COUNTIF(F5:G5,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>AND(COUNTIF(F5:G5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D5)))</formula>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>AND(XFD20&lt;&gt;"",NOT(A20&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="1" priority="5">
-      <formula>COUNTIF(F8:G8,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6">
-      <formula>AND(COUNTIF(F8:G8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D8)))</formula>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>COUNTIF(F18:G18,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>AND(COUNTIF(F18:G18,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B18 B21" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Number (per year)"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0200-000001000000}">
@@ -1056,5 +1259,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>